<commit_message>
added webdriver for mac
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24380" windowHeight="17120" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="17120" windowWidth="24380" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" sheetId="2" r:id="rId1"/>
-    <sheet name="TestSteps" sheetId="7" r:id="rId2"/>
-    <sheet name="TestData" sheetId="5" r:id="rId3"/>
-    <sheet name="Dictionary" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="TestCases" r:id="rId1" sheetId="2"/>
+    <sheet name="TestSteps" r:id="rId2" sheetId="7"/>
+    <sheet name="TestData" r:id="rId3" sheetId="5"/>
+    <sheet name="Dictionary" r:id="rId4" sheetId="4"/>
+    <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="80">
   <si>
     <t>Description</t>
   </si>
@@ -263,12 +263,16 @@
   </si>
   <si>
     <t>TS_7</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -311,27 +315,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -348,10 +352,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -515,21 +519,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -546,7 +550,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -598,29 +602,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.83203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.1640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.1640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.83203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1">
+    <row customFormat="1" r="1" s="2" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -644,10 +648,13 @@
       <c r="C2" t="s">
         <v>71</v>
       </c>
+      <c r="D2" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -657,21 +664,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="59.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.83203125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="59.5" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.83203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -716,6 +723,9 @@
       <c r="F2" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="G2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
@@ -733,6 +743,9 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
+      <c r="G3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
@@ -753,6 +766,9 @@
       <c r="F4" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="G4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
@@ -773,6 +789,9 @@
       <c r="F5" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="G5" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
@@ -791,6 +810,9 @@
         <v>7</v>
       </c>
       <c r="F6" s="7"/>
+      <c r="G6" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
@@ -811,6 +833,9 @@
       <c r="F7" s="8" t="s">
         <v>77</v>
       </c>
+      <c r="G7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
@@ -826,6 +851,9 @@
         <v>12</v>
       </c>
       <c r="F8"/>
+      <c r="G8" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="9" spans="1:7">
       <c r="D9" s="6"/>
@@ -837,7 +865,7 @@
       <c r="D11" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -847,8 +875,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -856,10 +884,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -945,7 +973,7 @@
       <c r="C18" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -955,8 +983,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -964,11 +992,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1">
+    <row customFormat="1" r="1" s="2" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -1032,7 +1060,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1042,8 +1070,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20:F20"/>
@@ -1051,7 +1079,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1306,7 +1334,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="84">
+    <row ht="84" r="20" spans="1:6">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -1327,7 +1355,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added constants.java and dataengine.xlsx
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -1,25 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aWorkspace\automation\src\dataEngine\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16500" windowHeight="2910" activeTab="1"/>
+    <workbookView activeTab="2" windowHeight="17800" windowWidth="26080" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" sheetId="2" r:id="rId1"/>
-    <sheet name="TestSteps" sheetId="7" r:id="rId2"/>
-    <sheet name="TestData" sheetId="5" r:id="rId3"/>
-    <sheet name="Dictionary" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="TestCases" r:id="rId1" sheetId="2"/>
+    <sheet name="TestSteps" r:id="rId2" sheetId="7"/>
+    <sheet name="TestData" r:id="rId3" sheetId="5"/>
+    <sheet name="Dictionary" r:id="rId4" sheetId="4"/>
+    <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="92">
   <si>
     <t>Description</t>
   </si>
@@ -252,9 +250,6 @@
     <t>openbrowser</t>
   </si>
   <si>
-    <t>Chrome</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -304,12 +299,16 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,27 +351,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -389,10 +388,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -427,7 +426,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -462,7 +461,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -556,21 +555,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -587,7 +586,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -639,29 +638,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.83203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.1640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -675,7 +674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -686,34 +685,39 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="59.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.1640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="59.5" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.83203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -736,7 +740,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -756,10 +760,10 @@
         <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -776,10 +780,10 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -799,12 +803,12 @@
         <v>25</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -822,10 +826,10 @@
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -843,10 +847,10 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -857,87 +861,87 @@
         <v>68</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>70</v>
       </c>
       <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="C8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
         <v>68</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s">
         <v>53</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -947,56 +951,56 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
         <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" t="s">
         <v>53</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1006,29 +1010,37 @@
         <v>12</v>
       </c>
       <c r="F14" s="8"/>
+      <c r="G14" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -1042,7 +1054,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -1053,10 +1065,10 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -1070,66 +1082,71 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -1137,80 +1154,85 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -1224,7 +1246,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -1238,7 +1260,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>59</v>
       </c>
@@ -1252,7 +1274,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -1266,7 +1288,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -1280,7 +1302,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1294,7 +1316,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -1308,7 +1330,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -1322,7 +1344,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -1336,7 +1358,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -1350,7 +1372,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -1364,7 +1386,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>60</v>
       </c>
@@ -1378,7 +1400,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -1392,7 +1414,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -1406,7 +1428,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>60</v>
       </c>
@@ -1420,7 +1442,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1434,7 +1456,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>60</v>
       </c>
@@ -1448,7 +1470,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -1462,7 +1484,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row ht="84" r="20" spans="1:6">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -1483,6 +1505,11 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
at pc, added constants.java, dataengine.xlsx, log4j2
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aWorkspace\automation\src\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16500" windowHeight="2910" activeTab="1"/>
+    <workbookView activeTab="1" windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" sheetId="2" r:id="rId1"/>
-    <sheet name="TestSteps" sheetId="7" r:id="rId2"/>
-    <sheet name="TestData" sheetId="5" r:id="rId3"/>
-    <sheet name="Dictionary" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="TestCases" r:id="rId1" sheetId="2"/>
+    <sheet name="TestSteps" r:id="rId2" sheetId="7"/>
+    <sheet name="TestData" r:id="rId3" sheetId="5"/>
+    <sheet name="Dictionary" r:id="rId4" sheetId="4"/>
+    <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="92">
   <si>
     <t>Description</t>
   </si>
@@ -310,6 +310,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,27 +353,27 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -389,10 +390,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -427,7 +428,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -462,7 +463,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -556,21 +557,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -587,7 +588,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -639,15 +640,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -655,13 +656,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -690,27 +691,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="59.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="59.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1006,15 +1007,18 @@
         <v>12</v>
       </c>
       <c r="F14" s="8"/>
+      <c r="G14" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
@@ -1022,10 +1026,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,13 +1115,13 @@
       <c r="C18" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -1125,11 +1129,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -1193,13 +1197,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20:F20"/>
@@ -1207,7 +1211,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1462,7 +1466,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -1483,6 +1487,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
enable prefix for testData keywords that need to refer to testData sheet
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="2" windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" r:id="rId1" sheetId="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="94">
   <si>
     <t>Description</t>
   </si>
@@ -246,9 +246,6 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Browser</t>
-  </si>
-  <si>
     <t>openbrowser</t>
   </si>
   <si>
@@ -304,6 +301,15 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>d_browser</t>
+  </si>
+  <si>
+    <t>d_username</t>
+  </si>
+  <si>
+    <t>d_password</t>
   </si>
 </sst>
 </file>
@@ -687,7 +693,7 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -700,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,13 +757,13 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -777,7 +783,7 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -797,15 +803,15 @@
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="G4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -820,10 +826,10 @@
         <v>8</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -844,7 +850,7 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -858,16 +864,16 @@
         <v>68</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -875,20 +881,20 @@
         <v>70</v>
       </c>
       <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="C8" t="s">
-        <v>80</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="8"/>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -896,18 +902,18 @@
         <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F9" s="8"/>
       <c r="G9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -915,22 +921,22 @@
         <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
         <v>68</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E10" t="s">
         <v>53</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -938,7 +944,7 @@
         <v>70</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -948,7 +954,7 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -956,17 +962,17 @@
         <v>70</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -974,22 +980,22 @@
         <v>70</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
         <v>68</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" t="s">
         <v>53</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -997,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1008,7 +1014,7 @@
       </c>
       <c r="F14" s="8"/>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1020,16 +1026,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1037,13 +1042,13 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>25</v>
+        <v>92</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1057,7 +1062,7 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated fetch_TestData function to able to read newly added columns in testData sheet; make logger look better for html; deleted logger for start and end; refactor getCellData function
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="95">
   <si>
     <t>Description</t>
   </si>
@@ -310,6 +310,9 @@
   </si>
   <si>
     <t>d_password</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
added keyword verifyURL, selectDropDown, tryNavigate
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
+    <workbookView windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" r:id="rId1" sheetId="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="109">
   <si>
     <t>Description</t>
   </si>
@@ -261,9 +261,6 @@
     <t>log keluar</t>
   </si>
   <si>
-    <t>TS_7</t>
-  </si>
-  <si>
     <t>//*[@id="page-container"]/div[5]/input[1]</t>
   </si>
   <si>
@@ -282,37 +279,82 @@
     <t>android</t>
   </si>
   <si>
-    <t>TS_8</t>
-  </si>
-  <si>
-    <t>TS_9</t>
-  </si>
-  <si>
-    <t>TS_10</t>
-  </si>
-  <si>
-    <t>TS_11</t>
-  </si>
-  <si>
-    <t>TS_12</t>
-  </si>
-  <si>
-    <t>TS_13</t>
+    <t>d_browser</t>
+  </si>
+  <si>
+    <t>d_username</t>
+  </si>
+  <si>
+    <t>d_password</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>other</t>
+  </si>
+  <si>
+    <t>verifyDownload</t>
+  </si>
+  <si>
+    <t>click deposit tab</t>
+  </si>
+  <si>
+    <t>//*[@id="page-container"]/div[4]/div[1]/div/div[1]/div/a/img</t>
+  </si>
+  <si>
+    <t>//*[@id="DepositBankList"]</t>
+  </si>
+  <si>
+    <t>select dropdown</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>//*[@id="tbAmount"]</t>
+  </si>
+  <si>
+    <t>input deposit amount</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>//*[@id="btnSubmitDeposit"]</t>
+  </si>
+  <si>
+    <t>http://directpay.besthappylife.biz/Pages/h2p/Login.aspx</t>
+  </si>
+  <si>
+    <t>verify URL</t>
+  </si>
+  <si>
+    <t>verifyURL</t>
+  </si>
+  <si>
+    <t>navigate back</t>
+  </si>
+  <si>
+    <t>tryNavigate</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>deposit page</t>
+  </si>
+  <si>
+    <t>deposit</t>
+  </si>
+  <si>
+    <t>download page</t>
   </si>
   <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>d_browser</t>
-  </si>
-  <si>
-    <t>d_username</t>
-  </si>
-  <si>
-    <t>d_password</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -320,7 +362,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,6 +385,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -361,10 +411,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -377,8 +428,11 @@
     <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
     <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -657,15 +711,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="21.85546875" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="12.140625" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="28.140625" collapsed="true"/>
@@ -696,7 +750,46 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -707,19 +800,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="59.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.85546875" collapsed="true"/>
   </cols>
   <sheetData>
@@ -763,10 +856,10 @@
         <v>72</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G2" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -786,7 +879,7 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -806,10 +899,10 @@
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -829,10 +922,10 @@
         <v>8</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -853,7 +946,7 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -876,78 +969,69 @@
         <v>76</v>
       </c>
       <c r="G7" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>77</v>
-      </c>
-      <c r="C8" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>78</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="8"/>
-      <c r="G8" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="6"/>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>68</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E10" t="s">
         <v>53</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>86</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>11</v>
@@ -955,35 +1039,28 @@
       <c r="E11" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F11"/>
-      <c r="G11" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G12" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>88</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
         <v>68</v>
@@ -997,30 +1074,156 @@
       <c r="F13" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="G13" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
         <v>89</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G15" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" t="s">
+        <v>94</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="9" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" t="s">
-        <v>90</v>
+      <c r="F20" s="8"/>
+      <c r="G20" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D18"/>
+  </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -1029,13 +1232,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
     <col min="2" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
@@ -1045,13 +1248,13 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1070,7 +1273,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>41</v>
@@ -1083,14 +1286,23 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>106</v>
+      </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>104</v>
+      </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>

</xml_diff>

<commit_message>
run once when there is no testData existed for the test case
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aWorkspace\automation\src\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16500" windowHeight="2910"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" r:id="rId1" sheetId="2"/>
-    <sheet name="TestSteps" r:id="rId2" sheetId="7"/>
-    <sheet name="TestData" r:id="rId3" sheetId="5"/>
-    <sheet name="Dictionary" r:id="rId4" sheetId="4"/>
-    <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
+    <sheet name="TestCases" sheetId="2" r:id="rId1"/>
+    <sheet name="TestSteps" sheetId="7" r:id="rId2"/>
+    <sheet name="TestData" sheetId="5" r:id="rId3"/>
+    <sheet name="Dictionary" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="122">
   <si>
     <t>Description</t>
   </si>
@@ -348,62 +348,58 @@
     <t>download page</t>
   </si>
   <si>
+    <t>loginMY</t>
+  </si>
+  <si>
+    <t>TS_7</t>
+  </si>
+  <si>
+    <t>TS_8</t>
+  </si>
+  <si>
+    <t>TS_9</t>
+  </si>
+  <si>
+    <t>TS_10</t>
+  </si>
+  <si>
+    <t>TS_11</t>
+  </si>
+  <si>
+    <t>TS_12</t>
+  </si>
+  <si>
+    <t>TS_13</t>
+  </si>
+  <si>
+    <t>TS_14</t>
+  </si>
+  <si>
+    <t>TS_15</t>
+  </si>
+  <si>
+    <t>TS_16</t>
+  </si>
+  <si>
+    <t>TS_17</t>
+  </si>
+  <si>
+    <t>TS_18</t>
+  </si>
+  <si>
+    <t>TS_19</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>loginMY</t>
-  </si>
-  <si>
     <t>loginEN</t>
-  </si>
-  <si>
-    <t>TS_7</t>
-  </si>
-  <si>
-    <t>TS_8</t>
-  </si>
-  <si>
-    <t>TS_9</t>
-  </si>
-  <si>
-    <t>TS_10</t>
-  </si>
-  <si>
-    <t>TS_11</t>
-  </si>
-  <si>
-    <t>TS_12</t>
-  </si>
-  <si>
-    <t>TS_13</t>
-  </si>
-  <si>
-    <t>TS_14</t>
-  </si>
-  <si>
-    <t>TS_15</t>
-  </si>
-  <si>
-    <t>TS_16</t>
-  </si>
-  <si>
-    <t>TS_17</t>
-  </si>
-  <si>
-    <t>TS_18</t>
-  </si>
-  <si>
-    <t>TS_19</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -454,31 +450,31 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -495,10 +491,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -533,7 +529,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -568,7 +564,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -662,21 +658,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -693,7 +689,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -745,29 +741,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="28.140625" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -783,7 +779,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
         <v>58</v>
@@ -792,70 +788,70 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D5" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="59.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.85546875" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="59.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -883,7 +879,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -901,12 +897,12 @@
         <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -921,12 +917,12 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -944,12 +940,12 @@
         <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -967,12 +963,12 @@
         <v>84</v>
       </c>
       <c r="G5" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -988,12 +984,12 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
@@ -1011,7 +1007,7 @@
         <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1019,7 +1015,7 @@
         <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
         <v>87</v>
@@ -1031,7 +1027,7 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1039,7 +1035,7 @@
         <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C9" t="s">
         <v>90</v>
@@ -1054,7 +1050,7 @@
         <v>91</v>
       </c>
       <c r="G9" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1062,7 +1058,7 @@
         <v>104</v>
       </c>
       <c r="B10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
         <v>93</v>
@@ -1077,7 +1073,7 @@
         <v>94</v>
       </c>
       <c r="G10" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1085,7 +1081,7 @@
         <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -1097,7 +1093,7 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1105,7 +1101,7 @@
         <v>104</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
         <v>97</v>
@@ -1117,7 +1113,7 @@
         <v>98</v>
       </c>
       <c r="G12" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1125,7 +1121,7 @@
         <v>104</v>
       </c>
       <c r="B13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C13" t="s">
         <v>99</v>
@@ -1137,7 +1133,7 @@
         <v>101</v>
       </c>
       <c r="G13" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1145,7 +1141,7 @@
         <v>102</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
@@ -1156,7 +1152,7 @@
       </c>
       <c r="F14" s="8"/>
       <c r="G14" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1164,7 +1160,7 @@
         <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
         <v>77</v>
@@ -1182,7 +1178,7 @@
         <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C16" t="s">
         <v>78</v>
@@ -1198,7 +1194,7 @@
         <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C17" t="s">
         <v>68</v>
@@ -1218,7 +1214,7 @@
         <v>86</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
@@ -1232,7 +1228,7 @@
         <v>86</v>
       </c>
       <c r="B19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C19" t="s">
         <v>78</v>
@@ -1247,7 +1243,7 @@
         <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C20" t="s">
         <v>68</v>
@@ -1264,25 +1260,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D12"/>
+    <hyperlink ref="D12" r:id="rId1"/>
   </hyperlinks>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1301,7 +1297,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -1315,7 +1311,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>41</v>
@@ -1327,29 +1323,14 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>102</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -1357,11 +1338,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" r="1" s="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -1425,13 +1406,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20:F20"/>
@@ -1439,7 +1420,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1694,7 +1675,7 @@
         <v>57</v>
       </c>
     </row>
-    <row ht="45" r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -1715,6 +1696,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
make the checking to function check_IfGotTestData
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aWorkspace\automation\src\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16500" windowHeight="2910"/>
+    <workbookView activeTab="2" windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCases" sheetId="2" r:id="rId1"/>
-    <sheet name="TestSteps" sheetId="7" r:id="rId2"/>
-    <sheet name="TestData" sheetId="5" r:id="rId3"/>
-    <sheet name="Dictionary" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId5"/>
+    <sheet name="TestCases" r:id="rId1" sheetId="2"/>
+    <sheet name="TestSteps" r:id="rId2" sheetId="7"/>
+    <sheet name="TestData" r:id="rId3" sheetId="5"/>
+    <sheet name="Dictionary" r:id="rId4" sheetId="4"/>
+    <sheet name="Sheet1" r:id="rId5" sheetId="6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -390,16 +390,17 @@
     <t>TS_19</t>
   </si>
   <si>
+    <t>loginEN</t>
+  </si>
+  <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>loginEN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -450,31 +451,31 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -491,10 +492,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -529,7 +530,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -564,7 +565,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -658,21 +659,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -689,7 +690,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -741,29 +742,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="28.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -788,7 +789,7 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -802,7 +803,7 @@
         <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -816,7 +817,7 @@
         <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -831,27 +832,27 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="59.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="59.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -897,7 +898,7 @@
         <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -917,7 +918,7 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -940,7 +941,7 @@
         <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -963,7 +964,7 @@
         <v>84</v>
       </c>
       <c r="G5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -984,7 +985,7 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1007,7 +1008,7 @@
         <v>75</v>
       </c>
       <c r="G7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1027,7 +1028,7 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1050,7 +1051,7 @@
         <v>91</v>
       </c>
       <c r="G9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1073,7 +1074,7 @@
         <v>94</v>
       </c>
       <c r="G10" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1093,7 +1094,7 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1113,7 +1114,7 @@
         <v>98</v>
       </c>
       <c r="G12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1133,7 +1134,7 @@
         <v>101</v>
       </c>
       <c r="G13" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1152,7 +1153,7 @@
       </c>
       <c r="F14" s="8"/>
       <c r="G14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1260,25 +1261,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D12" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="D12"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="12.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="2" max="3" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,7 +1312,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>41</v>
@@ -1324,13 +1325,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -1338,11 +1339,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" r="1" s="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
@@ -1406,13 +1407,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20:F20"/>
@@ -1420,7 +1421,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1675,7 +1676,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>70</v>
       </c>
@@ -1696,6 +1697,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added keyword trySlide function
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="2" windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" windowHeight="2910" windowWidth="16500" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" r:id="rId1" sheetId="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="169">
   <si>
     <t>Description</t>
   </si>
@@ -204,9 +204,6 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>Login into MS</t>
-  </si>
-  <si>
     <t>Login1</t>
   </si>
   <si>
@@ -270,12 +267,6 @@
     <t>trySwitch</t>
   </si>
   <si>
-    <t>/html/body/div/div[1]/div[2]/div/div[1]/h3</t>
-  </si>
-  <si>
-    <t>android</t>
-  </si>
-  <si>
     <t>d_browser</t>
   </si>
   <si>
@@ -285,115 +276,265 @@
     <t>d_password</t>
   </si>
   <si>
+    <t>verifyDownload</t>
+  </si>
+  <si>
+    <t>click deposit tab</t>
+  </si>
+  <si>
+    <t>//*[@id="page-container"]/div[4]/div[1]/div/div[1]/div/a/img</t>
+  </si>
+  <si>
+    <t>//*[@id="DepositBankList"]</t>
+  </si>
+  <si>
+    <t>select dropdown</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>//*[@id="tbAmount"]</t>
+  </si>
+  <si>
+    <t>input deposit amount</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>//*[@id="btnSubmitDeposit"]</t>
+  </si>
+  <si>
+    <t>http://directpay.besthappylife.biz/Pages/h2p/Login.aspx</t>
+  </si>
+  <si>
+    <t>verify URL</t>
+  </si>
+  <si>
+    <t>verifyURL</t>
+  </si>
+  <si>
+    <t>navigate back</t>
+  </si>
+  <si>
+    <t>tryNavigate</t>
+  </si>
+  <si>
+    <t>back</t>
+  </si>
+  <si>
+    <t>close</t>
+  </si>
+  <si>
+    <t>deposit page</t>
+  </si>
+  <si>
+    <t>deposit</t>
+  </si>
+  <si>
+    <t>download page</t>
+  </si>
+  <si>
+    <t>loginMY</t>
+  </si>
+  <si>
+    <t>TS_7</t>
+  </si>
+  <si>
+    <t>TS_8</t>
+  </si>
+  <si>
+    <t>TS_9</t>
+  </si>
+  <si>
+    <t>TS_10</t>
+  </si>
+  <si>
+    <t>TS_11</t>
+  </si>
+  <si>
+    <t>TS_12</t>
+  </si>
+  <si>
+    <t>TS_13</t>
+  </si>
+  <si>
+    <t>TS_14</t>
+  </si>
+  <si>
+    <t>TS_15</t>
+  </si>
+  <si>
+    <t>TS_16</t>
+  </si>
+  <si>
+    <t>TS_17</t>
+  </si>
+  <si>
+    <t>TS_18</t>
+  </si>
+  <si>
+    <t>TS_19</t>
+  </si>
+  <si>
+    <t>loginEN</t>
+  </si>
+  <si>
+    <t>//*[@id="page-container"]/div[2]/div/div[2]/div[2]/div/a/div[2]</t>
+  </si>
+  <si>
+    <t>click change language</t>
+  </si>
+  <si>
+    <t>//*[@id="page-container"]/div[2]/div/div[2]/div[2]/div/div/div[2]/div/div[1]/a</t>
+  </si>
+  <si>
+    <t>click English</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>TS_20</t>
+  </si>
+  <si>
+    <t>TS_21</t>
+  </si>
+  <si>
+    <t>TS_22</t>
+  </si>
+  <si>
+    <t>TS_23</t>
+  </si>
+  <si>
+    <t>TS_24</t>
+  </si>
+  <si>
+    <t>TS_25</t>
+  </si>
+  <si>
+    <t>TS_26</t>
+  </si>
+  <si>
+    <t>TS_27</t>
+  </si>
+  <si>
+    <t>http://ms.scrpower99.com/</t>
+  </si>
+  <si>
+    <t>http://54.251.181.7:8099/</t>
+  </si>
+  <si>
+    <t>LiveChat</t>
+  </si>
+  <si>
+    <t>//*[@id="livechat-btn"]</t>
+  </si>
+  <si>
+    <t>click livechat button</t>
+  </si>
+  <si>
+    <t>https://secure.livechatinc.com/licence/6613181/open_chat.cgi?groups=1</t>
+  </si>
+  <si>
+    <t>//*[@id="page-container"]/div[4]/div[1]/div/div[5]/div/a/img</t>
+  </si>
+  <si>
+    <t>click contact button</t>
+  </si>
+  <si>
+    <t>//*[@id="myButton"]</t>
+  </si>
+  <si>
+    <t>click START button</t>
+  </si>
+  <si>
+    <t>TS_28</t>
+  </si>
+  <si>
+    <t>TS_29</t>
+  </si>
+  <si>
+    <t>TS_30</t>
+  </si>
+  <si>
+    <t>TS_31</t>
+  </si>
+  <si>
+    <t>TS_32</t>
+  </si>
+  <si>
+    <t>TS_33</t>
+  </si>
+  <si>
+    <t>TS_34</t>
+  </si>
+  <si>
+    <t>TS_35</t>
+  </si>
+  <si>
+    <t>TS_36</t>
+  </si>
+  <si>
+    <t>TS_37</t>
+  </si>
+  <si>
+    <t>TS_38</t>
+  </si>
+  <si>
     <t>no</t>
   </si>
   <si>
-    <t>verifyDownload</t>
-  </si>
-  <si>
-    <t>click deposit tab</t>
-  </si>
-  <si>
-    <t>//*[@id="page-container"]/div[4]/div[1]/div/div[1]/div/a/img</t>
-  </si>
-  <si>
-    <t>//*[@id="DepositBankList"]</t>
-  </si>
-  <si>
-    <t>select dropdown</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>//*[@id="tbAmount"]</t>
-  </si>
-  <si>
-    <t>input deposit amount</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>//*[@id="btnSubmitDeposit"]</t>
-  </si>
-  <si>
-    <t>http://directpay.besthappylife.biz/Pages/h2p/Login.aspx</t>
-  </si>
-  <si>
-    <t>verify URL</t>
-  </si>
-  <si>
-    <t>verifyURL</t>
-  </si>
-  <si>
-    <t>navigate back</t>
-  </si>
-  <si>
-    <t>tryNavigate</t>
-  </si>
-  <si>
-    <t>back</t>
-  </si>
-  <si>
-    <t>close</t>
-  </si>
-  <si>
-    <t>deposit page</t>
-  </si>
-  <si>
-    <t>deposit</t>
-  </si>
-  <si>
-    <t>download page</t>
-  </si>
-  <si>
-    <t>loginMY</t>
-  </si>
-  <si>
-    <t>TS_7</t>
-  </si>
-  <si>
-    <t>TS_8</t>
-  </si>
-  <si>
-    <t>TS_9</t>
-  </si>
-  <si>
-    <t>TS_10</t>
-  </si>
-  <si>
-    <t>TS_11</t>
-  </si>
-  <si>
-    <t>TS_12</t>
-  </si>
-  <si>
-    <t>TS_13</t>
-  </si>
-  <si>
-    <t>TS_14</t>
-  </si>
-  <si>
-    <t>TS_15</t>
-  </si>
-  <si>
-    <t>TS_16</t>
-  </si>
-  <si>
-    <t>TS_17</t>
-  </si>
-  <si>
-    <t>TS_18</t>
-  </si>
-  <si>
-    <t>TS_19</t>
-  </si>
-  <si>
-    <t>loginEN</t>
+    <t>liveChat</t>
+  </si>
+  <si>
+    <t>verify liveChat page</t>
+  </si>
+  <si>
+    <t>ServiceAdv</t>
+  </si>
+  <si>
+    <t>//*[@id="sAdvantageOwl"]/div[1]/div/div[1]/div/div[1]</t>
+  </si>
+  <si>
+    <t>serviceAdv</t>
+  </si>
+  <si>
+    <t>TS_39</t>
+  </si>
+  <si>
+    <t>deposit masa nyata</t>
+  </si>
+  <si>
+    <t>slide</t>
+  </si>
+  <si>
+    <t>trySlide</t>
+  </si>
+  <si>
+    <t>TS_40</t>
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>//*[@id="sAdvantageOwl"]/div[1]/div/div[2]/div/div[1]</t>
+  </si>
+  <si>
+    <t>pengeluaran masa nyata</t>
+  </si>
+  <si>
+    <t>TS_41</t>
+  </si>
+  <si>
+    <t>TS_42</t>
+  </si>
+  <si>
+    <t>//*[@id="sAdvantageOwl"]/div[1]/div/div[1]/div/div[2]/div[3]/table/tbody/tr[1]/td[3]</t>
+  </si>
+  <si>
+    <t>-700</t>
   </si>
 </sst>
 </file>
@@ -750,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,55 +921,94 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D4" t="s">
-        <v>121</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -839,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,9 +1030,9 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="59.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="46.42578125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="12.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -880,7 +1060,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -892,18 +1072,18 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G2" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
@@ -912,18 +1092,18 @@
         <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
@@ -932,21 +1112,21 @@
         <v>5</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
@@ -955,21 +1135,21 @@
         <v>4</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -978,290 +1158,675 @@
         <v>6</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
         <v>53</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G7" t="s">
-        <v>121</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>2</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" t="s">
-        <v>121</v>
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" t="s">
         <v>104</v>
       </c>
-      <c r="B9" t="s">
-        <v>108</v>
-      </c>
       <c r="C9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G9" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10" t="s">
-        <v>121</v>
+        <v>120</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" t="s">
         <v>7</v>
-      </c>
-      <c r="G11" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" t="s">
-        <v>121</v>
+        <v>5</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G13" t="s">
-        <v>121</v>
+        <v>4</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="8"/>
-      <c r="G14" t="s">
-        <v>121</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B15" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="8"/>
+        <v>53</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
+        <v>11</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" t="s">
-        <v>79</v>
+      <c r="E16" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C17" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>81</v>
+        <v>84</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" t="s">
         <v>86</v>
       </c>
-      <c r="B18" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>12</v>
+      <c r="D18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="9" t="s">
-        <v>79</v>
+        <v>89</v>
+      </c>
+      <c r="D19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>122</v>
+      </c>
+      <c r="C21" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
+        <v>129</v>
+      </c>
+      <c r="C28" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" t="s">
+        <v>94</v>
+      </c>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B29" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>132</v>
+      </c>
+      <c r="B30" t="s">
+        <v>141</v>
+      </c>
+      <c r="C30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>132</v>
+      </c>
+      <c r="B31" t="s">
+        <v>142</v>
+      </c>
+      <c r="C31" t="s">
+        <v>93</v>
+      </c>
+      <c r="D31" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>132</v>
+      </c>
+      <c r="B32" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" t="s">
+        <v>144</v>
+      </c>
+      <c r="C33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34" t="s">
+        <v>145</v>
+      </c>
+      <c r="C34" t="s">
+        <v>137</v>
+      </c>
+      <c r="D34" t="s">
+        <v>136</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" t="s">
+        <v>146</v>
+      </c>
+      <c r="C35" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" t="s">
+        <v>138</v>
+      </c>
+      <c r="E35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" t="s">
+        <v>147</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" t="s">
+        <v>93</v>
+      </c>
+      <c r="D37" t="s">
+        <v>135</v>
+      </c>
+      <c r="E37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>132</v>
+      </c>
+      <c r="B38" t="s">
+        <v>149</v>
+      </c>
+      <c r="C38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>154</v>
+      </c>
+      <c r="B40" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>71</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>154</v>
+      </c>
+      <c r="B41" t="s">
+        <v>161</v>
+      </c>
+      <c r="C41" t="s">
+        <v>67</v>
+      </c>
+      <c r="D41" t="s">
+        <v>155</v>
+      </c>
+      <c r="E41" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>75</v>
+      <c r="F41" t="s">
+        <v>158</v>
+      </c>
+      <c r="G41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" t="s">
+        <v>165</v>
+      </c>
+      <c r="C42" t="s">
+        <v>159</v>
+      </c>
+      <c r="D42" t="s">
+        <v>167</v>
+      </c>
+      <c r="E42" t="s">
+        <v>160</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G42" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>154</v>
+      </c>
+      <c r="B43" t="s">
+        <v>166</v>
+      </c>
+      <c r="C43" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G43" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="D12"/>
+    <hyperlink r:id="rId1" ref="D21"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -1269,10 +1834,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,18 +1852,18 @@
         <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -1307,12 +1872,12 @@
         <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>41</v>
@@ -1321,6 +1886,14 @@
         <v>27</v>
       </c>
       <c r="D3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>154</v>
+      </c>
+      <c r="D4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1393,12 +1966,12 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1435,12 +2008,12 @@
         <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>35</v>
@@ -1454,7 +2027,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>36</v>
@@ -1468,7 +2041,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>37</v>
@@ -1482,7 +2055,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>38</v>
@@ -1496,7 +2069,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>39</v>
@@ -1510,7 +2083,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>40</v>
@@ -1524,7 +2097,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>41</v>
@@ -1538,7 +2111,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>42</v>
@@ -1552,7 +2125,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>43</v>
@@ -1566,7 +2139,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
@@ -1580,7 +2153,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>44</v>
@@ -1594,7 +2167,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>45</v>
@@ -1608,7 +2181,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>46</v>
@@ -1622,7 +2195,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>47</v>
@@ -1636,7 +2209,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>48</v>
@@ -1650,7 +2223,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>49</v>
@@ -1664,7 +2237,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>50</v>
@@ -1678,16 +2251,16 @@
     </row>
     <row ht="45" r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
       <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>69</v>
       </c>
       <c r="E20" t="s">
         <v>53</v>

</xml_diff>

<commit_message>
added keyword tryScroll function
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="173">
   <si>
     <t>Description</t>
   </si>
@@ -535,6 +535,18 @@
   </si>
   <si>
     <t>-700</t>
+  </si>
+  <si>
+    <t>scroll down</t>
+  </si>
+  <si>
+    <t>tryScroll</t>
+  </si>
+  <si>
+    <t>TS_43</t>
+  </si>
+  <si>
+    <t>//*[@id="sAdvantageOwl"]/div[1]/div/div[1]/div/div[2]/div[1]/table/tbody/tr[1]/td[2]/b</t>
   </si>
 </sst>
 </file>
@@ -1019,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,7 +1637,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -1639,7 +1651,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -1656,7 +1668,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>132</v>
       </c>
@@ -1673,7 +1685,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>132</v>
       </c>
@@ -1687,7 +1699,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>132</v>
       </c>
@@ -1704,7 +1716,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>132</v>
       </c>
@@ -1718,7 +1730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>132</v>
       </c>
@@ -1732,7 +1744,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>154</v>
       </c>
@@ -1755,7 +1767,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>154</v>
       </c>
@@ -1778,7 +1790,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -1786,22 +1798,20 @@
         <v>165</v>
       </c>
       <c r="C42" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="D42" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E42" t="s">
-        <v>160</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>168</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="F42"/>
       <c r="G42" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>154</v>
       </c>
@@ -1809,18 +1819,41 @@
         <v>166</v>
       </c>
       <c r="C43" t="s">
+        <v>159</v>
+      </c>
+      <c r="D43" t="s">
+        <v>167</v>
+      </c>
+      <c r="E43" t="s">
+        <v>160</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G43" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>154</v>
+      </c>
+      <c r="B44" t="s">
+        <v>171</v>
+      </c>
+      <c r="C44" t="s">
         <v>67</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>163</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E44" t="s">
         <v>53</v>
       </c>
-      <c r="F43" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G44" t="s">
         <v>162</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit before trying to install maven
</commit_message>
<xml_diff>
--- a/src/dataEngine/DataEngine.xlsx
+++ b/src/dataEngine/DataEngine.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="258">
   <si>
     <t>Description</t>
   </si>
@@ -604,9 +604,6 @@
   </si>
   <si>
     <t>zaq12wsx</t>
-  </si>
-  <si>
-    <t>http://ms.scrpower99.com/DepositResult/7fab428a-933f-4df9-b17e-55f73008df1a/success</t>
   </si>
   <si>
     <t>//*[@id="page-container"]/div[5]/div[8]/input</t>
@@ -787,7 +784,28 @@
     <t>PASS</t>
   </si>
   <si>
+    <t>//*[@id="page-container"]/div[5]/div[7]</t>
+  </si>
+  <si>
+    <t>TS_64</t>
+  </si>
+  <si>
+    <t>wait until it shows</t>
+  </si>
+  <si>
     <t>FAIL</t>
+  </si>
+  <si>
+    <t>wait until the web element show</t>
+  </si>
+  <si>
+    <t>web element to wait</t>
+  </si>
+  <si>
+    <t>NULL, clickable</t>
+  </si>
+  <si>
+    <t>Taraf：Siap</t>
   </si>
 </sst>
 </file>
@@ -795,7 +813,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,6 +844,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -848,7 +872,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
@@ -873,6 +897,7 @@
     <xf applyAlignment="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1190,7 +1215,7 @@
         <v>182</v>
       </c>
       <c r="D2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1204,7 +1229,7 @@
         <v>182</v>
       </c>
       <c r="D3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1215,7 +1240,7 @@
         <v>182</v>
       </c>
       <c r="D4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1298,7 +1323,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C14" t="s">
         <v>142</v>
@@ -1312,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,7 +1396,7 @@
         <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1391,7 +1416,7 @@
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1414,7 +1439,7 @@
         <v>73</v>
       </c>
       <c r="G4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1437,7 +1462,7 @@
         <v>74</v>
       </c>
       <c r="G5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1458,7 +1483,7 @@
       </c>
       <c r="F6" s="12"/>
       <c r="G6" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1481,7 +1506,7 @@
         <v>67</v>
       </c>
       <c r="G7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1649,7 +1674,7 @@
       </c>
       <c r="F16" s="13"/>
       <c r="G16" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2181,7 +2206,7 @@
         <v>6</v>
       </c>
       <c r="G47" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2192,19 +2217,19 @@
         <v>178</v>
       </c>
       <c r="C48" t="s">
+        <v>204</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>205</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>206</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>51</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G48" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2218,13 +2243,13 @@
         <v>185</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G49" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2235,19 +2260,19 @@
         <v>180</v>
       </c>
       <c r="C50" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>51</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G50" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2270,7 +2295,7 @@
         <v>80</v>
       </c>
       <c r="G51" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2293,7 +2318,7 @@
         <v>83</v>
       </c>
       <c r="G52" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -2301,7 +2326,7 @@
         <v>91</v>
       </c>
       <c r="B53" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -2313,7 +2338,7 @@
         <v>6</v>
       </c>
       <c r="G53" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -2321,7 +2346,7 @@
         <v>91</v>
       </c>
       <c r="B54" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C54" t="s">
         <v>86</v>
@@ -2333,7 +2358,7 @@
         <v>87</v>
       </c>
       <c r="G54" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -2341,13 +2366,13 @@
         <v>91</v>
       </c>
       <c r="B55" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C55" t="s">
         <v>186</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E55" s="8" t="s">
         <v>7</v>
@@ -2356,7 +2381,7 @@
         <v>190</v>
       </c>
       <c r="G55" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -2364,13 +2389,13 @@
         <v>91</v>
       </c>
       <c r="B56" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C56" t="s">
         <v>187</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>7</v>
@@ -2379,7 +2404,7 @@
         <v>191</v>
       </c>
       <c r="G56" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -2387,19 +2412,19 @@
         <v>91</v>
       </c>
       <c r="B57" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C57" t="s">
         <v>188</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G57" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -2407,19 +2432,19 @@
         <v>91</v>
       </c>
       <c r="B58" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C58" t="s">
-        <v>189</v>
+        <v>252</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>192</v>
+        <v>250</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>87</v>
+        <v>170</v>
       </c>
       <c r="G58" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -2427,70 +2452,79 @@
         <v>91</v>
       </c>
       <c r="B59" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C59" t="s">
-        <v>194</v>
-      </c>
-      <c r="D59" t="s">
-        <v>193</v>
+        <v>189</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>250</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>88</v>
+        <v>51</v>
+      </c>
+      <c r="F59" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="G59" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>238</v>
+        <v>91</v>
       </c>
       <c r="B60" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C60" t="s">
-        <v>2</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>239</v>
+        <v>193</v>
+      </c>
+      <c r="D60" t="s">
+        <v>192</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>64</v>
+        <v>6</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>53</v>
+        <v>88</v>
+      </c>
+      <c r="G60" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>237</v>
+      </c>
+      <c r="B61" t="s">
+        <v>244</v>
+      </c>
+      <c r="C61" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="9" t="s">
         <v>238</v>
       </c>
-      <c r="B61" t="s">
-        <v>245</v>
-      </c>
-      <c r="C61" t="s">
-        <v>241</v>
-      </c>
-      <c r="D61" t="s">
-        <v>240</v>
-      </c>
       <c r="E61" s="8" t="s">
-        <v>6</v>
+        <v>64</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B62" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C62" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D62" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>6</v>
@@ -2498,39 +2532,56 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B63" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C63" t="s">
-        <v>70</v>
+        <v>242</v>
+      </c>
+      <c r="D63" t="s">
+        <v>241</v>
       </c>
       <c r="E63" s="8" t="s">
-        <v>71</v>
+        <v>6</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B64" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C64" t="s">
+        <v>70</v>
+      </c>
+      <c r="E64" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>237</v>
+      </c>
+      <c r="B65" t="s">
+        <v>251</v>
+      </c>
+      <c r="C65" t="s">
         <v>158</v>
       </c>
-      <c r="D64" t="s">
-        <v>248</v>
-      </c>
-      <c r="E64" s="8" t="s">
+      <c r="D65" t="s">
+        <v>247</v>
+      </c>
+      <c r="E65" s="8" t="s">
         <v>159</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="D54"/>
-    <hyperlink r:id="rId2" ref="D60"/>
+    <hyperlink r:id="rId2" ref="D61"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9" r:id="rId3"/>
@@ -2617,15 +2668,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="31.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="28.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
@@ -2647,156 +2698,170 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
         <v>64</v>
       </c>
       <c r="C2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" t="s">
         <v>212</v>
-      </c>
-      <c r="D2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D3" t="s">
         <v>215</v>
-      </c>
-      <c r="D3" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" t="s">
         <v>218</v>
-      </c>
-      <c r="D4" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B5" t="s">
         <v>51</v>
       </c>
       <c r="C5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>221</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B7" t="s">
         <v>52</v>
       </c>
       <c r="C7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>225</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B8" t="s">
         <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>228</v>
+      </c>
+      <c r="B9" t="s">
         <v>229</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9" t="s">
         <v>230</v>
-      </c>
-      <c r="C9" t="s">
-        <v>216</v>
-      </c>
-      <c r="D9" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B10" t="s">
         <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B11" t="s">
         <v>159</v>
       </c>
       <c r="C11" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D11" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B12" t="s">
         <v>151</v>
       </c>
       <c r="C12" t="s">
+        <v>235</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>237</v>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" t="s">
+        <v>255</v>
+      </c>
+      <c r="D13" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>